<commit_message>
1.1 arbitrary number of stimuli exemplars, no longer fixed to 5
Separated block structure and stimuli exemplars into separate excel
files and applied a shuffle()/pop() method first employed in the IRAP
R script updated appropriately.
</commit_message>
<xml_diff>
--- a/stimuli.xlsx
+++ b/stimuli.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500"/>
@@ -22,10 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
-  <si>
-    <t>trialtype</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>flower1.jpg</t>
   </si>
@@ -93,10 +90,28 @@
     <t>insect5.jpg</t>
   </si>
   <si>
-    <t>stimulusText</t>
-  </si>
-  <si>
-    <t>stimulusImage</t>
+    <t>text_trial_type_1_exemplars</t>
+  </si>
+  <si>
+    <t>text_trial_type_2_exemplars</t>
+  </si>
+  <si>
+    <t>text_trial_type_3_exemplars</t>
+  </si>
+  <si>
+    <t>text_trial_type_4_exemplars</t>
+  </si>
+  <si>
+    <t>img_trial_type_1_exemplars</t>
+  </si>
+  <si>
+    <t>img_trial_type_2_exemplars</t>
+  </si>
+  <si>
+    <t>img_trial_type_3_exemplars</t>
+  </si>
+  <si>
+    <t>img_trial_type_4_exemplars</t>
   </si>
 </sst>
 </file>
@@ -142,36 +157,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF7B9B6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF68DFA8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF1890A8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF244B88"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -183,7 +174,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="213">
+  <cellStyleXfs count="239">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -397,43 +388,51 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="213">
+  <cellStyles count="239">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -540,6 +539,19 @@
     <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -646,6 +658,19 @@
     <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -975,21 +1000,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.5" customWidth="1"/>
-    <col min="2" max="3" width="13.5" style="1" customWidth="1"/>
+    <col min="1" max="2" width="24.6640625" style="6" customWidth="1"/>
+    <col min="3" max="4" width="24.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="24.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>23</v>
@@ -997,229 +1024,153 @@
       <c r="C1" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="2">
+    <row r="2" spans="1:8">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
+      <c r="F3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3" t="s">
+    <row r="4" spans="1:8">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="F4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="2">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="3" t="s">
+    <row r="5" spans="1:8">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="F5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="2">
-        <v>1</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="3" t="s">
+    <row r="6" spans="1:8">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="2">
-        <v>1</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="F6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="2">
-        <v>2</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="2">
-        <v>2</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="2">
-        <v>2</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="2">
-        <v>2</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="2">
-        <v>2</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="2">
-        <v>3</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="2">
-        <v>3</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="2">
-        <v>3</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="2">
-        <v>3</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="2">
-        <v>3</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="2">
-        <v>4</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="2">
-        <v>4</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="2">
-        <v>4</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="2">
-        <v>4</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="2">
-        <v>4</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>6</v>
+      <c r="H6" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>